<commit_message>
cleaned data, updated stats
</commit_message>
<xml_diff>
--- a/lessthan25.xlsx
+++ b/lessthan25.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="1800" windowWidth="25600" windowHeight="18400" tabRatio="500"/>
+    <workbookView xWindow="5160" yWindow="1920" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="lessthan25.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -123,12 +123,6 @@
     <t xml:space="preserve">these are people with "too much data" </t>
   </si>
   <si>
-    <t>need mouth AOI data</t>
-  </si>
-  <si>
-    <t>added to finaladultdata.csv</t>
-  </si>
-  <si>
     <t>data is correct, this story should be dropped during nb03</t>
   </si>
   <si>
@@ -141,35 +135,44 @@
     <t>rv4</t>
   </si>
   <si>
-    <t>added to finaladultdata.csv but need to compare with Lynette</t>
-  </si>
-  <si>
-    <t>added to finaladultdata.csv; check if still good or not</t>
-  </si>
-  <si>
-    <t>actually in group 2; fixed in finaladultdata.csv; check if still good or not</t>
-  </si>
-  <si>
-    <t>data is correct. maybe in wrong group?</t>
-  </si>
-  <si>
     <t>Josh - rv2 King Midas - total AOIs = 40.21 (but story is 37s)</t>
   </si>
   <si>
-    <t>need rv2 data again</t>
-  </si>
-  <si>
-    <t>need fw1 data again</t>
-  </si>
-  <si>
     <t>thick glasses</t>
+  </si>
+  <si>
+    <t>data updated in finaladultdata.csv, fixed!</t>
+  </si>
+  <si>
+    <t>glasses, I guess…</t>
+  </si>
+  <si>
+    <t>seems out of range</t>
+  </si>
+  <si>
+    <t>don't know why, quirk?</t>
+  </si>
+  <si>
+    <t>added to finaladultdata.csv, good</t>
+  </si>
+  <si>
+    <t>added to finaladultdata.csv, kinda low</t>
+  </si>
+  <si>
+    <t>added to finaladultdata.csv, looks good now</t>
+  </si>
+  <si>
+    <t>added to finaladultdata.csv, still low</t>
+  </si>
+  <si>
+    <t>data is correct. Dunno…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,8 +204,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,12 +220,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,8 +245,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -283,10 +309,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -303,6 +329,18 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -319,6 +357,18 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,264 +701,264 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1">
-      <c r="A2" s="3">
+    <row r="2" spans="1:10" s="2" customFormat="1">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1">
-      <c r="A3" s="3">
+    <row r="3" spans="1:10" s="2" customFormat="1">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="3" customFormat="1">
-      <c r="A4" s="3">
+    <row r="4" spans="1:10" s="2" customFormat="1">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1">
-      <c r="A5" s="3">
+    <row r="5" spans="1:10" s="2" customFormat="1">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="2">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
+    <row r="6" spans="1:10" s="1" customFormat="1">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1">
-      <c r="A7" s="4">
+      <c r="I6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1">
-      <c r="A8" s="4">
+      <c r="I7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>10</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4">
+      <c r="I8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
         <v>10</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>41</v>
+      <c r="I9" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -963,68 +1013,68 @@
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1">
-      <c r="A12" s="3">
+    <row r="12" spans="1:10" s="1" customFormat="1">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="4" customFormat="1">
-      <c r="A13" s="4">
+      <c r="J12" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="2" customFormat="1">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>6</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="2">
         <v>0</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>40</v>
+      <c r="I13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1">
@@ -1053,254 +1103,272 @@
         <v>3.8</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2.91</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2">
+        <v>4.62</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="G19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H15">
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
+      <c r="H19" s="2">
+        <v>6.84</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="3" customFormat="1">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3">
+        <v>30</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2.56</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H16">
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17">
-        <v>4.62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3">
-        <v>7</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.81</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="3">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="3">
-        <v>6.84</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="4" customFormat="1">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4">
+      <c r="H21" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1">
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="4" customFormat="1">
+      <c r="A28" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1">
+      <c r="B29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="2" customFormat="1">
+      <c r="B30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="3" customFormat="1">
+      <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="4">
-        <v>2.56</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="3" customFormat="1">
-      <c r="C22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="5" customFormat="1">
-      <c r="A28" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="I30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="4" customFormat="1">
-      <c r="B31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="4" customFormat="1">
-      <c r="B32" s="4" t="s">
+      <c r="I31" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="3" customFormat="1">
+      <c r="B32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" s="4" customFormat="1">
-      <c r="B33" s="4" t="s">
+      <c r="I32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" s="5" customFormat="1">
+      <c r="B33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="4" t="s">
-        <v>42</v>
+      <c r="I33" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>